<commit_message>
update nrf24L01P_module_PCB on my_lib_tiny
</commit_message>
<xml_diff>
--- a/boards/sae_son/BOM.xlsx
+++ b/boards/sae_son/BOM.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,19 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Documents\GitHub\designSpark\boards\sae_son\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{BBB0E4E5-FB58-4D8C-B066-4BE30E32A399}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8753A8E-075E-4394-BA04-86AC218E5A4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="44">
   <si>
     <t>Ref Name</t>
   </si>
@@ -146,12 +159,18 @@
   </si>
   <si>
     <t>Description</t>
+  </si>
+  <si>
+    <t>ok</t>
+  </si>
+  <si>
+    <t>ok des 74HC14</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -487,7 +506,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -617,6 +636,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -662,12 +692,14 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20 % - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1022,11 +1054,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1036,7 +1068,7 @@
     <col min="6" max="6" width="38.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1056,7 +1088,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>9</v>
       </c>
@@ -1075,8 +1107,11 @@
       <c r="F2" s="3" t="s">
         <v>39</v>
       </c>
+      <c r="G2" s="5" t="s">
+        <v>42</v>
+      </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>31</v>
       </c>
@@ -1093,8 +1128,11 @@
       <c r="F3" s="3" t="s">
         <v>37</v>
       </c>
+      <c r="G3" s="5" t="s">
+        <v>42</v>
+      </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>16</v>
       </c>
@@ -1112,7 +1150,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>32</v>
       </c>
@@ -1129,8 +1167,11 @@
       <c r="F5" s="4" t="s">
         <v>35</v>
       </c>
+      <c r="G5" s="6" t="s">
+        <v>42</v>
+      </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>22</v>
       </c>
@@ -1149,8 +1190,11 @@
       <c r="F6" s="4" t="s">
         <v>26</v>
       </c>
+      <c r="G6" s="6" t="s">
+        <v>42</v>
+      </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>33</v>
       </c>
@@ -1167,8 +1211,11 @@
       <c r="F7" s="4" t="s">
         <v>34</v>
       </c>
+      <c r="G7" s="6" t="s">
+        <v>42</v>
+      </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>27</v>
       </c>
@@ -1188,7 +1235,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>7</v>
       </c>
@@ -1205,8 +1252,11 @@
       <c r="F9" s="3" t="s">
         <v>38</v>
       </c>
+      <c r="G9" s="5" t="s">
+        <v>42</v>
+      </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>11</v>
       </c>
@@ -1222,6 +1272,9 @@
       <c r="E10" s="4"/>
       <c r="F10" s="4" t="s">
         <v>36</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>